<commit_message>
vault backup: 2025-12-06 12:58:32
</commit_message>
<xml_diff>
--- a/Strumenti/Strumenti.xlsx
+++ b/Strumenti/Strumenti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B152B-48B9-4C66-9024-2E935D219CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2690D43B-8FB3-4EC7-BEB9-E8B0C0FADD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9996" yWindow="504" windowWidth="31584" windowHeight="15228" activeTab="5" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="15396" yWindow="816" windowWidth="20988" windowHeight="13860" activeTab="1" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="_Malkavian" sheetId="19" r:id="rId1"/>
@@ -23033,31 +23033,31 @@
       </c>
       <c r="E3" s="36">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L3" s="36">
         <f t="shared" ca="1" si="0"/>
@@ -23065,7 +23065,7 @@
       </c>
       <c r="M3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N3" s="36"/>
     </row>
@@ -23112,23 +23112,23 @@
       </c>
       <c r="I5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -23158,23 +23158,23 @@
       </c>
       <c r="I6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -23200,27 +23200,27 @@
       </c>
       <c r="H7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -23246,7 +23246,7 @@
       </c>
       <c r="H8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I8" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23258,15 +23258,15 @@
       </c>
       <c r="K8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -23284,11 +23284,11 @@
       </c>
       <c r="F9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23296,7 +23296,7 @@
       </c>
       <c r="I9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23304,15 +23304,15 @@
       </c>
       <c r="K9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -23330,7 +23330,7 @@
       </c>
       <c r="F10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23338,7 +23338,7 @@
       </c>
       <c r="H10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23346,19 +23346,19 @@
       </c>
       <c r="J10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -23372,11 +23372,11 @@
       </c>
       <c r="E11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23388,7 +23388,7 @@
       </c>
       <c r="I11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23396,15 +23396,15 @@
       </c>
       <c r="K11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -23426,11 +23426,11 @@
       </c>
       <c r="G12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23438,19 +23438,19 @@
       </c>
       <c r="J12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -23472,11 +23472,11 @@
       </c>
       <c r="G13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="38">
         <f t="shared" ca="1" si="3"/>
@@ -23484,19 +23484,19 @@
       </c>
       <c r="J13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -23519,7 +23519,7 @@
       </c>
       <c r="G16" s="41" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -23535,7 +23535,7 @@
       <c r="F18" s="38"/>
       <c r="G18" s="42" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23561,7 +23561,7 @@
       <c r="F20" s="38"/>
       <c r="G20" s="42" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23587,7 +23587,7 @@
       <c r="F22" s="38"/>
       <c r="G22" s="42" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23600,7 +23600,7 @@
       <c r="F23" s="38"/>
       <c r="G23" s="42" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -25795,8 +25795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F8F40E-FA57-4F3C-B9C3-6981E5263578}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -34636,7 +34636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB020AF3-E2AF-4B08-9CF1-A8BB16CCBDFC}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>

</xml_diff>